<commit_message>
Add/Edit Python for ML
</commit_message>
<xml_diff>
--- a/Python For ML/myexcel.xlsx
+++ b/Python For ML/myexcel.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -431,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,193 +436,126 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>raw_grade</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>D</t>
+          <t>grade</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45580</v>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.39740659516181</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.04222396303112243</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-0.2210786148769942</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-0.0725167699240183</v>
+        <v>1</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>very good</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45581</v>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9837853525130844</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-1.652721420933177</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1.450148396505617</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-0.2781699554053059</v>
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45582</v>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-1.684738408612102</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.2923654135577397</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.265665391706035</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.214957075800284</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45583</v>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.4484605477188084</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.8067090090914775</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0.3816847702543433</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.09342212004498557</v>
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>very good</t>
+        </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45584</v>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>-1.576795903172302</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.3956191225650882</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.449044067865205</v>
-      </c>
-      <c r="E6" t="n">
-        <v>-0.5395239102346423</v>
+        <v>5</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>very good</t>
+        </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45585</v>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.03138772921028537</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1.120717865568175</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-0.8324696534796178</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.407241775099394</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>45586</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.6490916217359655</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1.421723295584337</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.263561114557161</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-0.5063306002096422</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45587</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.6399726016587501</v>
-      </c>
-      <c r="C9" t="n">
-        <v>-0.3334036630887126</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-1.0711090896924</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-0.8794056558159284</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>45588</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.3935132462003782</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.09505802958774576</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.1226700898234489</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.1463792687152566</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>45589</v>
-      </c>
-      <c r="B11" t="n">
-        <v>-0.1993892391299355</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.021882380044156</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.4906030023031735</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.9801031041746726</v>
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>e</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>very bad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>